<commit_message>
Improve Import of BLP Data: Resolve Redirects. Better Logging.
see https://redmine.informationgrid.eu/issues/994
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>id</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>http://www.langelsheim.de/Verwaltung-Politik/Rathaus/Bauleitplanung/Bebauungspl%C3%A4ne</t>
+  </si>
+  <si>
+    <t>Fürstenau, Samtgemeinde</t>
+  </si>
+  <si>
+    <t>http://www.fuerstenau.de/Aktuelles/Bekanntmachungen</t>
+  </si>
+  <si>
+    <t>Berge, Bippen, Stadt Fürstenau</t>
   </si>
 </sst>
 </file>
@@ -256,7 +265,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -578,396 +587,26 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>459403</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>52.5018461</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>7.6307787</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Ignore SSL certificate errors while analysing URLs.
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -11,14 +11,14 @@
     <sheet name="BLP-URLs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$404</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$405</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>descr</t>
+  </si>
+  <si>
+    <t>Juist, Inselgemeinde</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/0BxMfdWAA8UdsUFhRMzdDdnh4Z1E</t>
+  </si>
+  <si>
+    <t>http://www.gemeinde-juist.de/</t>
   </si>
   <si>
     <t>Braunschweig, Stadt</t>
@@ -262,10 +271,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -304,18 +313,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>101000</v>
+        <v>452013</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>52.26249</v>
+        <v>53.678347</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>10.520525</v>
+        <v>6.995328</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>8</v>
@@ -326,16 +335,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>102000</v>
+        <v>101000</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>52.160601</v>
+        <v>52.26249</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>10.328465</v>
+        <v>10.520525</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
@@ -346,110 +355,107 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>103000</v>
+        <v>102000</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>52.421938</v>
+        <v>52.160601</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>10.784975</v>
+        <v>10.328465</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>151009</v>
+        <v>103000</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>52.484369</v>
+        <v>52.421938</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>10.54687</v>
+        <v>10.784975</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>151040</v>
+        <v>151009</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>52.72877</v>
+        <v>52.484369</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>10.740212</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>10.54687</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>151401</v>
+        <v>151040</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>52.5064174</v>
+        <v>52.72877</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>10.7230508</v>
+        <v>10.740212</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="0" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>151402</v>
+        <v>151401</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>52.5870835</v>
+        <v>52.5064174</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>10.8261885</v>
+        <v>10.7230508</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>151403</v>
+        <v>151402</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>52.7145461</v>
+        <v>52.5870835</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>10.5739811</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>24</v>
+        <v>10.8261885</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>25</v>
@@ -457,16 +463,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>151404</v>
+        <v>151403</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>52.433333</v>
+        <v>52.7145461</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>10.5811443</v>
+        <v>10.5739811</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>27</v>
@@ -480,65 +486,65 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>151405</v>
+        <v>151404</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>52.4791352</v>
+        <v>52.433333</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>10.2595906</v>
+        <v>10.5811443</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>151406</v>
+        <v>151405</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>52.4791352</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>10.2595906</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>52.383333</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>10.5311443</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>151407</v>
+        <v>151406</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>52.383333</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>10.5311443</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>52.5961151</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>10.534286</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>38</v>
@@ -549,36 +555,39 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>153002</v>
+        <v>151407</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>51.880275</v>
+        <v>52.5961151</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>10.560048</v>
+        <v>10.534286</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>153007</v>
+        <v>153002</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>43</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>51.938286</v>
+        <v>51.880275</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>10.335897</v>
+        <v>10.560048</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>44</v>
@@ -587,24 +596,44 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>459403</v>
+        <v>153007</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>52.5018461</v>
+        <v>51.938286</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>7.6307787</v>
+        <v>10.335897</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>459403</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>52.5018461</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>7.6307787</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Handle redirect URLs starting with "../".
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -11,14 +11,14 @@
     <sheet name="BLP-URLs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$405</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$406</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>descr</t>
+  </si>
+  <si>
+    <t>Bad Iburg,Stadt</t>
+  </si>
+  <si>
+    <t>http://www.badiburg.de/bekanntmachungen</t>
   </si>
   <si>
     <t>Juist, Inselgemeinde</t>
@@ -271,7 +277,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
@@ -315,147 +321,147 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>452013</v>
+        <v>459004</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>53.678347</v>
+        <v>52.156471</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>6.995328</v>
+        <v>8.045253</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>452013</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>101000</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="n">
+        <v>53.678347</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6.995328</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>52.26249</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>10.520525</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>102000</v>
+        <v>101000</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>52.26249</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>10.520525</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>52.160601</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>10.328465</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>103000</v>
+        <v>102000</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>52.160601</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>10.328465</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>52.421938</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>10.784975</v>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>151009</v>
+        <v>103000</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>52.484369</v>
+        <v>52.421938</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>10.54687</v>
+        <v>10.784975</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>151040</v>
+        <v>151009</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>52.72877</v>
+        <v>52.484369</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>10.740212</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>20</v>
+        <v>10.54687</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>151401</v>
+        <v>151040</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>52.72877</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>10.740212</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>52.5064174</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>10.7230508</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="0" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>151402</v>
+        <v>151401</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>52.5064174</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>10.7230508</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>52.5870835</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>10.8261885</v>
+      <c r="F9" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>25</v>
@@ -463,177 +469,194 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>151403</v>
+        <v>151402</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>52.7145461</v>
+        <v>52.5870835</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>10.5739811</v>
-      </c>
-      <c r="E10" s="0" t="s">
+        <v>10.8261885</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>151404</v>
+        <v>151403</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>52.7145461</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>10.5739811</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>52.433333</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>10.5811443</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>151405</v>
+        <v>151404</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>52.433333</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>10.5811443</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>52.4791352</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>10.2595906</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>151406</v>
+        <v>151405</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>52.4791352</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>10.2595906</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>52.383333</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>10.5311443</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>151407</v>
+        <v>151406</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>52.383333</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>10.5311443</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>52.5961151</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>10.534286</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>153002</v>
+        <v>151407</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>52.5961151</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>10.534286</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>51.880275</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>10.560048</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
+        <v>153002</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>51.880275</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>10.560048</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
         <v>153007</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="0" t="n">
+      <c r="B17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>51.938286</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <v>10.335897</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="E17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
         <v>459403</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="0" t="n">
+      <c r="B18" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="0" t="n">
         <v>52.5018461</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>7.6307787</v>
       </c>
-      <c r="E17" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>51</v>
+      <c r="E18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More robust metadata refresh url extraction.
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -11,14 +11,14 @@
     <sheet name="BLP-URLs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$406</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$407</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>descr</t>
+  </si>
+  <si>
+    <t>Moormerland</t>
+  </si>
+  <si>
+    <t>http://www.mmld.de/download</t>
+  </si>
+  <si>
+    <t>http://lkleer.maps.arcgis.com/home/webmap/viewer.html?webmap=e4311f176259429d970921af4cf49ab2</t>
   </si>
   <si>
     <t>Bad Iburg,Stadt</t>
@@ -277,7 +286,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
@@ -321,53 +330,53 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>459004</v>
+        <v>457014</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>52.156471</v>
+        <v>53.314314</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>8.045253</v>
+        <v>7.485564</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>459004</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>52.156471</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>8.045253</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>452013</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>53.678347</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>6.995328</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>101000</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>52.26249</v>
+        <v>53.678347</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>10.520525</v>
+        <v>6.995328</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -378,16 +387,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>102000</v>
+        <v>101000</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>52.160601</v>
+        <v>52.26249</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>10.328465</v>
+        <v>10.520525</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>16</v>
@@ -398,110 +407,107 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>103000</v>
+        <v>102000</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>52.421938</v>
+        <v>52.160601</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>10.784975</v>
+        <v>10.328465</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>151009</v>
+        <v>103000</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>52.484369</v>
+        <v>52.421938</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>10.54687</v>
+        <v>10.784975</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>151040</v>
+        <v>151009</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>52.72877</v>
+        <v>52.484369</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>10.740212</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>22</v>
+        <v>10.54687</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>151401</v>
+        <v>151040</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>52.5064174</v>
+        <v>52.72877</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>10.7230508</v>
+        <v>10.740212</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="0" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>151402</v>
+        <v>151401</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>52.5870835</v>
+        <v>52.5064174</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>10.8261885</v>
+        <v>10.7230508</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>151403</v>
+        <v>151402</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>52.7145461</v>
+        <v>52.5870835</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>10.5739811</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>29</v>
+        <v>10.8261885</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>30</v>
@@ -509,16 +515,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>151404</v>
+        <v>151403</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>52.433333</v>
+        <v>52.7145461</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>10.5811443</v>
+        <v>10.5739811</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>32</v>
@@ -532,65 +538,65 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>151405</v>
+        <v>151404</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>52.4791352</v>
+        <v>52.433333</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>10.2595906</v>
+        <v>10.5811443</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>151406</v>
+        <v>151405</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>52.4791352</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>10.2595906</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>52.383333</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>10.5311443</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="G14" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>151407</v>
+        <v>151406</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>52.383333</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>10.5311443</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>52.5961151</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>10.534286</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>43</v>
@@ -601,36 +607,39 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>153002</v>
+        <v>151407</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>51.880275</v>
+        <v>52.5961151</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>10.560048</v>
+        <v>10.534286</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>46</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="0" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>153007</v>
+        <v>153002</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>51.938286</v>
+        <v>51.880275</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>10.335897</v>
+        <v>10.560048</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>49</v>
@@ -639,24 +648,44 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>459403</v>
+        <v>153007</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>52.5018461</v>
+        <v>51.938286</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>7.6307787</v>
+        <v>10.335897</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="F18" s="0" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>459403</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>52.5018461</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>7.6307787</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated blp-urls-test.xlsx from support 4.2.x branch (commit Release 4.2.3. !) Blame it, never committed to dev branch ! ;)
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -11,14 +11,14 @@
     <sheet name="BLP-URLs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$407</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$408</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>descr</t>
+  </si>
+  <si>
+    <t>Zetel</t>
+  </si>
+  <si>
+    <t>https://www.zetel.de/wirtschaft-bauen/bauleitplanung/amtliche-bekanntmachungen/</t>
+  </si>
+  <si>
+    <t>https://www.zetel.de/wirtschaft-bauen/bauleitplanung/bebauungsplaene-online/</t>
   </si>
   <si>
     <t>Moormerland</t>
@@ -264,7 +273,11 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,7 +299,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
@@ -328,75 +341,75 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>457014</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>455027</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>53.314314</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>7.485564</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="n">
+        <v>53.418096</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>7.973923</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>459004</v>
+        <v>457014</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>52.156471</v>
+        <v>53.314314</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>8.045253</v>
+        <v>7.485564</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
+        <v>459004</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>52.156471</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>8.045253</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
         <v>452013</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>53.678347</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>6.995328</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>101000</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>52.26249</v>
+        <v>53.678347</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>10.520525</v>
+        <v>6.995328</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>16</v>
@@ -407,16 +420,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>102000</v>
+        <v>101000</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>52.160601</v>
+        <v>52.26249</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>10.328465</v>
+        <v>10.520525</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>19</v>
@@ -427,110 +440,107 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>103000</v>
+        <v>102000</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>52.421938</v>
+        <v>52.160601</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>10.784975</v>
+        <v>10.328465</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>151009</v>
+        <v>103000</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>52.484369</v>
+        <v>52.421938</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>10.54687</v>
+        <v>10.784975</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>151040</v>
+        <v>151009</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>52.72877</v>
+        <v>52.484369</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>10.740212</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>25</v>
+        <v>10.54687</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>151401</v>
+        <v>151040</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>52.5064174</v>
+        <v>52.72877</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>10.7230508</v>
+        <v>10.740212</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>151402</v>
+        <v>151401</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>52.5870835</v>
+        <v>52.5064174</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>10.8261885</v>
+        <v>10.7230508</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>151403</v>
+        <v>151402</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>52.7145461</v>
+        <v>52.5870835</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>10.5739811</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>32</v>
+        <v>10.8261885</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>33</v>
@@ -538,16 +548,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>151404</v>
+        <v>151403</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>52.433333</v>
+        <v>52.7145461</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>10.5811443</v>
+        <v>10.5739811</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>35</v>
@@ -561,65 +571,65 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>151405</v>
+        <v>151404</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>52.4791352</v>
+        <v>52.433333</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>10.2595906</v>
+        <v>10.5811443</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>38</v>
       </c>
       <c r="F14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>151406</v>
+        <v>151405</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>52.4791352</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>10.2595906</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="0" t="n">
-        <v>52.383333</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>10.5311443</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="G15" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>151407</v>
+        <v>151406</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>52.383333</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>10.5311443</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>52.5961151</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>10.534286</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>46</v>
@@ -630,36 +640,39 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>153002</v>
+        <v>151407</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>51.880275</v>
+        <v>52.5961151</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>10.560048</v>
+        <v>10.534286</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>153007</v>
+        <v>153002</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>51.938286</v>
+        <v>51.880275</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>10.335897</v>
+        <v>10.560048</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>52</v>
@@ -668,24 +681,44 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>459403</v>
+        <v>153007</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>52.5018461</v>
+        <v>51.938286</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>7.6307787</v>
+        <v>10.335897</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>459403</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>52.5018461</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>7.6307787</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adapt excel parsing to the new excel file layout.
The excel table must have a specific layout. The first row must contain
the column names.
 
<ul>
<li>NAME: BLP name that appears on map popup as title.</li>
<li>LAT: LAT of map marker coordinate.</li>
<li>LON: LON of map marker coordinate.</li>
<li>URL_VERFAHREN_OFFEN: Url to BLPs in progress.</li>
<li>URL_VERFAHREN_ABGESCHLOSSEN: Url to finished BLPs.</li>
<li>MITGLIEDSGEMEINDEN: BLP description that appears on map popup.</li>
</ul>

Columns can be mixed. The excel file can contain other columns, as long
as the specified columns exist.

https://redmine.informationgrid.eu/issues/980
</commit_message>
<xml_diff>
--- a/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
+++ b/ingrid-iplug-se-iplug/src/test/resources/blp-urls-test.xlsx
@@ -11,34 +11,31 @@
     <sheet name="BLP-URLs" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$G$408</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'BLP-URLs'!$A$1:$F$408</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>url (im Verfahren)</t>
-  </si>
-  <si>
-    <t>url (abgeschlossen)</t>
-  </si>
-  <si>
-    <t>descr</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>URL_VERFAHREN_OFFEN</t>
+  </si>
+  <si>
+    <t>URL_VERFAHREN_ABGESCHLOSSEN</t>
+  </si>
+  <si>
+    <t>MITGLIEDSGEMEINDEN</t>
   </si>
   <si>
     <t>Zetel</t>
@@ -204,8 +201,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -273,12 +272,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -299,33 +302,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5748987854251"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2834008097166"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.4251012145749"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="76.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.4251012145749"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.1376518218624"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="76.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5748987854251"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -337,273 +339,231 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>455027</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="n">
+        <v>53.418096</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>7.973923</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>53.418096</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>7.973923</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>457014</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="0" t="n">
+        <v>53.314314</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>7.485564</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>53.314314</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>7.485564</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>459004</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="0" t="n">
+        <v>52.156471</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8.045253</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>52.156471</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>8.045253</v>
-      </c>
-      <c r="E4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>452013</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="0" t="n">
+        <v>53.678347</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>6.995328</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>53.678347</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>6.995328</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>101000</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="0" t="n">
+        <v>52.26249</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>10.520525</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>52.26249</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>10.520525</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>102000</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="0" t="n">
+        <v>52.160601</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>10.328465</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>52.160601</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>10.328465</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>103000</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="0" t="n">
+        <v>52.421938</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>10.784975</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>52.421938</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>10.784975</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>151009</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="0" t="n">
+        <v>52.484369</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>10.54687</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>52.484369</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>10.54687</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>151040</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="0" t="n">
+        <v>52.72877</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>10.740212</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>52.72877</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>10.740212</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>151401</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="0" t="n">
+        <v>52.5064174</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10.7230508</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="0" t="n">
-        <v>52.5064174</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>10.7230508</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>151402</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="0" t="n">
+        <v>52.5870835</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>10.8261885</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="0" t="n">
-        <v>52.5870835</v>
-      </c>
-      <c r="D12" s="0" t="n">
-        <v>10.8261885</v>
-      </c>
-      <c r="G12" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>151403</v>
-      </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="0" t="n">
+        <v>52.7145461</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>10.5739811</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="0" t="n">
-        <v>52.7145461</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>10.5739811</v>
-      </c>
       <c r="E13" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>151404</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="0" t="n">
+        <v>52.433333</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>10.5811443</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="0" t="n">
-        <v>52.433333</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>10.5811443</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>151405</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="0" t="n">
+        <v>52.4791352</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>10.2595906</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>52.4791352</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>10.2595906</v>
       </c>
       <c r="E15" s="0" t="s">
         <v>41</v>
@@ -611,22 +571,19 @@
       <c r="F15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="G15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>151406</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="0" t="n">
+        <v>52.383333</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>10.5311443</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>52.383333</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>10.5311443</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>45</v>
@@ -634,91 +591,76 @@
       <c r="F16" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>151407</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="0" t="n">
+        <v>52.5961151</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>10.534286</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="0" t="n">
-        <v>52.5961151</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>10.534286</v>
-      </c>
       <c r="E17" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G17" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>153002</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="0" t="n">
+        <v>51.880275</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>10.560048</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>51.880275</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>10.560048</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="0" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>153007</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="0" t="n">
+        <v>51.938286</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>10.335897</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" s="0" t="n">
-        <v>51.938286</v>
-      </c>
-      <c r="D19" s="0" t="n">
-        <v>10.335897</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="0" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>459403</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="0" t="n">
+        <v>52.5018461</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7.6307787</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="0" t="n">
-        <v>52.5018461</v>
-      </c>
-      <c r="D20" s="0" t="n">
-        <v>7.6307787</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="F20" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="G20" s="0" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>